<commit_message>
map stool to Stool
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@81448 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/Microbiome/doc/values_microbiome.xlsx
+++ b/Load/src/ontology/Microbiome/doc/values_microbiome.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15281" uniqueCount="1349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15282" uniqueCount="1349">
   <si>
     <t>Dwelling ID</t>
   </si>
@@ -4672,7 +4672,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4683,8 +4683,8 @@
   <dimension ref="A1:F6918"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F921" sqref="F921"/>
+      <pane ySplit="1" topLeftCell="A1172" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1181" sqref="E1181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -19918,7 +19918,9 @@
       <c r="C1182" t="s">
         <v>586</v>
       </c>
-      <c r="D1182" s="9"/>
+      <c r="D1182" s="9" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="1183" spans="1:4">
       <c r="A1183" t="s">

</xml_diff>